<commit_message>
Added environment variables from Jenkins.
</commit_message>
<xml_diff>
--- a/TestData/Custom_Quota.xlsx
+++ b/TestData/Custom_Quota.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9601BACD-E7EA-4ED3-8885-DAC18252974E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E540D744-0C7C-4E0D-94B5-94124A599EEB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -554,233 +554,6 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16.5">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="4">
-        <v>99999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1">
-        <v>50</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="1">
-        <v>99999</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-    </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
@@ -854,7 +627,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D03B8D5-BAB8-450E-A664-CABADEFF022A}">
-  <dimension ref="A24:C24"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD10"/>
@@ -870,10 +643,237 @@
     <col min="6" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="24" spans="1:3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+    <row r="1" spans="1:7" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="16.5">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="4">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1">
+        <v>50</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1">
+        <v>99999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes to improve performance
</commit_message>
<xml_diff>
--- a/TestData/Custom_Quota.xlsx
+++ b/TestData/Custom_Quota.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\STL_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2439A01-DD48-41C4-8B85-96C1BD6F7ECE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAD46D7-C2EF-4779-889D-3242A6D593CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="25995" windowHeight="13095" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
   <si>
     <t>${quota_name}</t>
   </si>
@@ -488,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B209AA-B2EF-4EBA-BC33-9B6FB480ED25}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -755,51 +755,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-    </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
@@ -819,6 +774,51 @@
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -828,10 +828,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D03B8D5-BAB8-450E-A664-CABADEFF022A}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A33:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD10"/>
+      <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -844,237 +844,10 @@
     <col min="6" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
-      <c r="A1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="16.5">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="4">
-        <v>99999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="1">
-        <v>50</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="1" customFormat="1">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1">
-        <v>99999</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>